<commit_message>
Remove electricity indicator from COMHET
</commit_message>
<xml_diff>
--- a/VT_IE_COM.xlsx
+++ b/VT_IE_COM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1132EE22-93BF-4101-9871-F92D47FE9193}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2E11BD-9E75-4A31-9562-7CC68C19A4D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="891" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="891" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="33" r:id="rId1"/>
@@ -1674,7 +1674,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1548" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="651">
   <si>
     <t>ELC</t>
   </si>
@@ -2833,9 +2833,6 @@
   </si>
   <si>
     <t>Particulate Matter &lt;2.5 µm (COM)</t>
-  </si>
-  <si>
-    <t>HEAT</t>
   </si>
   <si>
     <t>Commercial services</t>
@@ -9599,7 +9596,7 @@
     </row>
     <row r="17" spans="1:14" ht="102.75" customHeight="1">
       <c r="A17" s="787" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B17" s="787"/>
       <c r="C17" s="787"/>
@@ -9641,10 +9638,10 @@
     </row>
     <row r="20" spans="1:14" ht="17.25" customHeight="1">
       <c r="A20" s="421" t="s">
+        <v>406</v>
+      </c>
+      <c r="B20" s="788" t="s">
         <v>407</v>
-      </c>
-      <c r="B20" s="788" t="s">
-        <v>408</v>
       </c>
       <c r="C20" s="788"/>
       <c r="D20" s="788"/>
@@ -9661,10 +9658,10 @@
     </row>
     <row r="21" spans="1:14" ht="17.25" customHeight="1">
       <c r="A21" s="421" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B21" s="789" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C21" s="789"/>
       <c r="D21" s="789"/>
@@ -9681,10 +9678,10 @@
     </row>
     <row r="22" spans="1:14" ht="17.25" customHeight="1">
       <c r="A22" s="421" t="s">
+        <v>409</v>
+      </c>
+      <c r="B22" s="789" t="s">
         <v>410</v>
-      </c>
-      <c r="B22" s="789" t="s">
-        <v>411</v>
       </c>
       <c r="C22" s="789"/>
       <c r="D22" s="789"/>
@@ -9693,7 +9690,7 @@
     </row>
     <row r="23" spans="1:14" ht="17.25" customHeight="1">
       <c r="A23" s="424" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B23" s="577"/>
       <c r="C23" s="577"/>
@@ -9705,7 +9702,7 @@
     </row>
     <row r="24" spans="1:14" ht="17.25" customHeight="1">
       <c r="A24" s="790" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B24" s="790"/>
       <c r="C24" s="790"/>
@@ -9717,7 +9714,7 @@
     </row>
     <row r="25" spans="1:14" ht="17.25" customHeight="1">
       <c r="A25" s="786" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B25" s="786"/>
       <c r="C25" s="786"/>
@@ -9892,7 +9889,7 @@
   <dimension ref="B1:W177"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9900,7 +9897,7 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="12.86328125" customWidth="1"/>
     <col min="3" max="3" width="18.3984375" customWidth="1"/>
-    <col min="4" max="4" width="82.3984375" customWidth="1"/>
+    <col min="4" max="4" width="45.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1328125" bestFit="1" customWidth="1"/>
@@ -9934,7 +9931,7 @@
     </row>
     <row r="4" spans="2:22" s="16" customFormat="1" ht="14.25">
       <c r="B4" s="68" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G4" s="122" t="s">
         <v>236</v>
@@ -10033,7 +10030,7 @@
     </row>
     <row r="10" spans="2:22" s="16" customFormat="1" ht="18">
       <c r="B10" s="66" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C10" s="64"/>
       <c r="D10" s="64"/>
@@ -10057,7 +10054,7 @@
     </row>
     <row r="11" spans="2:22" s="16" customFormat="1" ht="14.25">
       <c r="C11" s="68" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="2:22" s="16" customFormat="1" ht="16.149999999999999" thickBot="1">
@@ -10065,61 +10062,61 @@
         <v>17</v>
       </c>
       <c r="C12" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="D12" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="F12" s="97" t="s">
         <v>557</v>
       </c>
-      <c r="D12" s="96" t="s">
-        <v>574</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>575</v>
-      </c>
-      <c r="F12" s="97" t="s">
+      <c r="G12" s="97" t="s">
         <v>558</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="H12" s="97" t="s">
         <v>559</v>
       </c>
-      <c r="H12" s="97" t="s">
+      <c r="I12" s="97" t="s">
         <v>560</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="J12" s="97" t="s">
         <v>561</v>
       </c>
-      <c r="J12" s="97" t="s">
+      <c r="K12" s="97" t="s">
         <v>562</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="L12" s="97" t="s">
         <v>563</v>
       </c>
-      <c r="L12" s="97" t="s">
+      <c r="M12" s="97" t="s">
         <v>564</v>
       </c>
-      <c r="M12" s="97" t="s">
+      <c r="N12" s="97" t="s">
         <v>565</v>
       </c>
-      <c r="N12" s="97" t="s">
+      <c r="O12" s="97" t="s">
         <v>566</v>
       </c>
-      <c r="O12" s="97" t="s">
+      <c r="P12" s="97" t="s">
         <v>567</v>
       </c>
-      <c r="P12" s="97" t="s">
+      <c r="Q12" s="97" t="s">
         <v>568</v>
       </c>
-      <c r="Q12" s="97" t="s">
+      <c r="R12" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="R12" s="97" t="s">
+      <c r="S12" s="97" t="s">
         <v>570</v>
       </c>
-      <c r="S12" s="97" t="s">
+      <c r="T12" s="97" t="s">
         <v>571</v>
       </c>
-      <c r="T12" s="97" t="s">
+      <c r="U12" s="97" t="s">
         <v>572</v>
-      </c>
-      <c r="U12" s="97" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="13" spans="2:22" s="16" customFormat="1" ht="14.25">
@@ -10128,13 +10125,13 @@
         <v>CHCS</v>
       </c>
       <c r="C13" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D13" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="E13" s="54" t="s">
         <v>577</v>
-      </c>
-      <c r="E13" s="54" t="s">
-        <v>578</v>
       </c>
       <c r="F13" s="589">
         <v>0.10037907809223</v>
@@ -10191,13 +10188,13 @@
         <v>CHPS</v>
       </c>
       <c r="C14" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D14" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="E14" s="54" t="s">
         <v>577</v>
-      </c>
-      <c r="E14" s="54" t="s">
-        <v>578</v>
       </c>
       <c r="F14" s="589">
         <v>0.10037907809223</v>
@@ -13738,7 +13735,7 @@
     <col min="1" max="1" width="5" style="16" customWidth="1"/>
     <col min="2" max="2" width="12.86328125" style="16" customWidth="1"/>
     <col min="3" max="3" width="20.3984375" style="16" customWidth="1"/>
-    <col min="4" max="4" width="58.86328125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.86328125" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1328125" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="12" width="12.59765625" style="16" customWidth="1"/>
     <col min="13" max="13" width="12.59765625" style="1" customWidth="1"/>
@@ -13785,7 +13782,7 @@
     </row>
     <row r="4" spans="2:23">
       <c r="B4" s="68" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F4" s="75"/>
       <c r="G4" s="122" t="s">
@@ -13944,7 +13941,7 @@
     </row>
     <row r="10" spans="2:23" ht="18">
       <c r="B10" s="66" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C10" s="64"/>
       <c r="D10" s="64"/>
@@ -13968,7 +13965,7 @@
     </row>
     <row r="11" spans="2:23">
       <c r="C11" s="68" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="M11" s="16"/>
       <c r="T11" s="16"/>
@@ -13979,61 +13976,61 @@
         <v>17</v>
       </c>
       <c r="C12" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="D12" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="F12" s="97" t="s">
         <v>557</v>
       </c>
-      <c r="D12" s="96" t="s">
-        <v>574</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>575</v>
-      </c>
-      <c r="F12" s="97" t="s">
+      <c r="G12" s="97" t="s">
         <v>558</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="H12" s="97" t="s">
         <v>559</v>
       </c>
-      <c r="H12" s="97" t="s">
+      <c r="I12" s="97" t="s">
         <v>560</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="J12" s="97" t="s">
         <v>561</v>
       </c>
-      <c r="J12" s="97" t="s">
+      <c r="K12" s="97" t="s">
         <v>562</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="L12" s="97" t="s">
         <v>563</v>
       </c>
-      <c r="L12" s="97" t="s">
+      <c r="M12" s="97" t="s">
         <v>564</v>
       </c>
-      <c r="M12" s="97" t="s">
+      <c r="N12" s="97" t="s">
         <v>565</v>
       </c>
-      <c r="N12" s="97" t="s">
+      <c r="O12" s="97" t="s">
         <v>566</v>
       </c>
-      <c r="O12" s="97" t="s">
+      <c r="P12" s="97" t="s">
         <v>567</v>
       </c>
-      <c r="P12" s="97" t="s">
+      <c r="Q12" s="97" t="s">
         <v>568</v>
       </c>
-      <c r="Q12" s="97" t="s">
+      <c r="R12" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="R12" s="97" t="s">
+      <c r="S12" s="97" t="s">
         <v>570</v>
       </c>
-      <c r="S12" s="97" t="s">
+      <c r="T12" s="97" t="s">
         <v>571</v>
       </c>
-      <c r="T12" s="97" t="s">
+      <c r="U12" s="97" t="s">
         <v>572</v>
-      </c>
-      <c r="U12" s="97" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="13" spans="2:23">
@@ -14042,13 +14039,13 @@
         <v>CWCS</v>
       </c>
       <c r="C13" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D13" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D13" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E13" s="54" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F13" s="589">
         <v>0.107921172700168</v>
@@ -14105,13 +14102,13 @@
         <v>CWPS</v>
       </c>
       <c r="C14" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D14" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D14" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E14" s="54" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F14" s="589">
         <v>0.107921172700168</v>
@@ -16616,7 +16613,7 @@
     <col min="1" max="1" width="5.1328125" customWidth="1"/>
     <col min="2" max="2" width="13.86328125" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.265625" customWidth="1"/>
     <col min="6" max="21" width="11.1328125" customWidth="1"/>
     <col min="22" max="255" width="11.3984375" customWidth="1"/>
@@ -16643,7 +16640,7 @@
     </row>
     <row r="4" spans="2:21" s="16" customFormat="1" ht="14.25">
       <c r="B4" s="68" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G4" s="122" t="s">
         <v>236</v>
@@ -16781,7 +16778,7 @@
     </row>
     <row r="10" spans="2:21" s="16" customFormat="1" ht="18">
       <c r="B10" s="66" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C10" s="64"/>
       <c r="D10" s="64"/>
@@ -16805,7 +16802,7 @@
     </row>
     <row r="11" spans="2:21" s="16" customFormat="1" ht="14.25">
       <c r="C11" s="68" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="12" spans="2:21" s="16" customFormat="1" ht="16.149999999999999" thickBot="1">
@@ -16813,61 +16810,61 @@
         <v>17</v>
       </c>
       <c r="C12" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="D12" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="E12" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="F12" s="97" t="s">
         <v>557</v>
       </c>
-      <c r="D12" s="96" t="s">
-        <v>574</v>
-      </c>
-      <c r="E12" s="96" t="s">
-        <v>575</v>
-      </c>
-      <c r="F12" s="97" t="s">
+      <c r="G12" s="97" t="s">
         <v>558</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="H12" s="97" t="s">
         <v>559</v>
       </c>
-      <c r="H12" s="97" t="s">
+      <c r="I12" s="97" t="s">
         <v>560</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="J12" s="97" t="s">
         <v>561</v>
       </c>
-      <c r="J12" s="97" t="s">
+      <c r="K12" s="97" t="s">
         <v>562</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="L12" s="97" t="s">
         <v>563</v>
       </c>
-      <c r="L12" s="97" t="s">
+      <c r="M12" s="97" t="s">
         <v>564</v>
       </c>
-      <c r="M12" s="97" t="s">
+      <c r="N12" s="97" t="s">
         <v>565</v>
       </c>
-      <c r="N12" s="97" t="s">
+      <c r="O12" s="97" t="s">
         <v>566</v>
       </c>
-      <c r="O12" s="97" t="s">
+      <c r="P12" s="97" t="s">
         <v>567</v>
       </c>
-      <c r="P12" s="97" t="s">
+      <c r="Q12" s="97" t="s">
         <v>568</v>
       </c>
-      <c r="Q12" s="97" t="s">
+      <c r="R12" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="R12" s="97" t="s">
+      <c r="S12" s="97" t="s">
         <v>570</v>
       </c>
-      <c r="S12" s="97" t="s">
+      <c r="T12" s="97" t="s">
         <v>571</v>
       </c>
-      <c r="T12" s="97" t="s">
+      <c r="U12" s="97" t="s">
         <v>572</v>
-      </c>
-      <c r="U12" s="97" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="13" spans="2:21" s="16" customFormat="1" ht="14.25">
@@ -16876,13 +16873,13 @@
         <v>CCCS</v>
       </c>
       <c r="C13" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D13" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D13" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E13" s="54" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F13" s="589">
         <v>0.14219999999999999</v>
@@ -16939,13 +16936,13 @@
         <v>CCPS</v>
       </c>
       <c r="C14" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D14" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D14" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E14" s="54" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F14" s="589">
         <v>0.14219999999999999</v>
@@ -18701,7 +18698,7 @@
   </sheetPr>
   <dimension ref="B1:X100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -18755,7 +18752,7 @@
     </row>
     <row r="4" spans="2:21" s="16" customFormat="1" ht="14.25">
       <c r="B4" s="68" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G4" s="122" t="s">
         <v>236</v>
@@ -18994,7 +18991,7 @@
     </row>
     <row r="13" spans="2:21" s="16" customFormat="1" ht="18">
       <c r="B13" s="66" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C13" s="64"/>
       <c r="D13" s="64"/>
@@ -19018,7 +19015,7 @@
     </row>
     <row r="14" spans="2:21" s="16" customFormat="1" ht="14.25">
       <c r="C14" s="68" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="15" spans="2:21" s="16" customFormat="1" ht="16.149999999999999" thickBot="1">
@@ -19026,61 +19023,61 @@
         <v>17</v>
       </c>
       <c r="C15" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="D15" s="96" t="s">
+        <v>573</v>
+      </c>
+      <c r="E15" s="96" t="s">
+        <v>574</v>
+      </c>
+      <c r="F15" s="97" t="s">
         <v>557</v>
       </c>
-      <c r="D15" s="96" t="s">
-        <v>574</v>
-      </c>
-      <c r="E15" s="96" t="s">
-        <v>575</v>
-      </c>
-      <c r="F15" s="97" t="s">
+      <c r="G15" s="97" t="s">
         <v>558</v>
       </c>
-      <c r="G15" s="97" t="s">
+      <c r="H15" s="97" t="s">
         <v>559</v>
       </c>
-      <c r="H15" s="97" t="s">
+      <c r="I15" s="97" t="s">
         <v>560</v>
       </c>
-      <c r="I15" s="97" t="s">
+      <c r="J15" s="97" t="s">
         <v>561</v>
       </c>
-      <c r="J15" s="97" t="s">
+      <c r="K15" s="97" t="s">
         <v>562</v>
       </c>
-      <c r="K15" s="97" t="s">
+      <c r="L15" s="97" t="s">
         <v>563</v>
       </c>
-      <c r="L15" s="97" t="s">
+      <c r="M15" s="97" t="s">
         <v>564</v>
       </c>
-      <c r="M15" s="97" t="s">
+      <c r="N15" s="97" t="s">
         <v>565</v>
       </c>
-      <c r="N15" s="97" t="s">
+      <c r="O15" s="97" t="s">
         <v>566</v>
       </c>
-      <c r="O15" s="97" t="s">
+      <c r="P15" s="97" t="s">
         <v>567</v>
       </c>
-      <c r="P15" s="97" t="s">
+      <c r="Q15" s="97" t="s">
         <v>568</v>
       </c>
-      <c r="Q15" s="97" t="s">
+      <c r="R15" s="97" t="s">
         <v>569</v>
       </c>
-      <c r="R15" s="97" t="s">
+      <c r="S15" s="97" t="s">
         <v>570</v>
       </c>
-      <c r="S15" s="97" t="s">
+      <c r="T15" s="97" t="s">
         <v>571</v>
       </c>
-      <c r="T15" s="97" t="s">
+      <c r="U15" s="97" t="s">
         <v>572</v>
-      </c>
-      <c r="U15" s="97" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="16" spans="2:21" s="16" customFormat="1" ht="14.25">
@@ -19089,13 +19086,13 @@
         <v>CLIG</v>
       </c>
       <c r="C16" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D16" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D16" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E16" s="54" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F16" s="589">
         <v>0.1125</v>
@@ -19152,13 +19149,13 @@
         <v>CCOK</v>
       </c>
       <c r="C17" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D17" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D17" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E17" s="54" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F17" s="589">
         <v>0.15</v>
@@ -19215,13 +19212,13 @@
         <v>CREF</v>
       </c>
       <c r="C18" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D18" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D18" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E18" s="54" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F18" s="589">
         <v>0.104166666666667</v>
@@ -19278,13 +19275,13 @@
         <v>CPLI</v>
       </c>
       <c r="C19" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D19" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D19" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E19" s="54" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F19" s="589">
         <v>0.1125</v>
@@ -19341,13 +19338,13 @@
         <v>COEL</v>
       </c>
       <c r="C20" s="54" t="s">
+        <v>575</v>
+      </c>
+      <c r="D20" s="54" t="s">
         <v>576</v>
       </c>
-      <c r="D20" s="54" t="s">
-        <v>577</v>
-      </c>
       <c r="E20" s="54" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F20" s="589">
         <v>0.104166666666667</v>
@@ -19425,13 +19422,13 @@
       <c r="P22" s="134"/>
       <c r="Q22" s="85"/>
       <c r="S22" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="T22" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="T22" s="16" t="s">
+      <c r="U22" s="16" t="s">
         <v>496</v>
-      </c>
-      <c r="U22" s="16" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="23" spans="2:24" s="16" customFormat="1" ht="29.25" thickBot="1">
@@ -19532,7 +19529,7 @@
         <v>133</v>
       </c>
       <c r="X24" s="470" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="25" spans="2:24" s="16" customFormat="1" ht="14.25">
@@ -21629,7 +21626,7 @@
         <v>246</v>
       </c>
       <c r="G7" s="782" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H7" s="186" t="s">
         <v>81</v>
@@ -21682,10 +21679,10 @@
     </row>
     <row r="9" spans="2:15" s="16" customFormat="1" ht="14.25">
       <c r="B9" s="140" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C9" s="140" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D9" s="54" t="s">
         <v>70</v>
@@ -21813,30 +21810,30 @@
   <sheetData>
     <row r="4" spans="2:9">
       <c r="I4" s="429" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="2:9">
       <c r="B5" s="430"/>
       <c r="C5" s="431" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="431" t="s">
         <v>414</v>
       </c>
-      <c r="D5" s="431" t="s">
+      <c r="E5" s="431" t="s">
         <v>415</v>
       </c>
-      <c r="E5" s="431" t="s">
+      <c r="F5" s="431" t="s">
         <v>416</v>
       </c>
-      <c r="F5" s="431" t="s">
+      <c r="G5" s="431" t="s">
         <v>417</v>
-      </c>
-      <c r="G5" s="431" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="432" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C6" s="433">
         <v>42283</v>
@@ -21856,7 +21853,7 @@
     </row>
     <row r="7" spans="2:9">
       <c r="B7" s="432" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C7" s="434">
         <v>0.39</v>
@@ -21874,12 +21871,12 @@
         <v>0.03</v>
       </c>
       <c r="I7" s="429" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="432" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C8" s="762">
         <f>'CSO data'!C36</f>
@@ -21902,12 +21899,12 @@
         <v>3365</v>
       </c>
       <c r="I8" s="768" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="432" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C9" s="480">
         <f>(SUM(C19:C21)*1000000000)/(C8*C6)</f>
@@ -21932,7 +21929,7 @@
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="432" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C10" s="433">
         <v>85140.600241231703</v>
@@ -21952,7 +21949,7 @@
     </row>
     <row r="11" spans="2:9" ht="28.5">
       <c r="B11" s="432" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C11" s="433">
         <v>40205.283447248308</v>
@@ -21981,7 +21978,7 @@
     </row>
     <row r="13" spans="2:9" ht="28.5">
       <c r="B13" s="430" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C13" s="431"/>
       <c r="D13" s="431"/>
@@ -21992,7 +21989,7 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="437" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C14" s="438">
         <v>0.21555878668166398</v>
@@ -22012,7 +22009,7 @@
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="437" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C15" s="438">
         <v>2.9381909961317933E-2</v>
@@ -22060,7 +22057,7 @@
     </row>
     <row r="18" spans="2:9" ht="42.75">
       <c r="B18" s="430" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C18" s="439"/>
       <c r="D18" s="439"/>
@@ -22068,12 +22065,12 @@
       <c r="F18" s="439"/>
       <c r="G18" s="439"/>
       <c r="I18" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="19" spans="2:9">
       <c r="B19" s="437" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C19" s="441">
         <v>3</v>
@@ -22091,12 +22088,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I19" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="437" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C20" s="441">
         <v>0.2</v>
@@ -22114,7 +22111,7 @@
         <v>0.6</v>
       </c>
       <c r="I20" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="2:9">
@@ -22137,7 +22134,7 @@
         <v>0.4</v>
       </c>
       <c r="I21" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="22" spans="2:9">
@@ -22150,7 +22147,7 @@
     </row>
     <row r="23" spans="2:9" ht="42.75">
       <c r="B23" s="430" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C23" s="439"/>
       <c r="D23" s="439"/>
@@ -22158,12 +22155,12 @@
       <c r="F23" s="439"/>
       <c r="G23" s="439"/>
       <c r="I23" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="437" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C24" s="435">
         <v>1.3</v>
@@ -22181,12 +22178,12 @@
         <v>0.9</v>
       </c>
       <c r="I24" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="437" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C25" s="435">
         <v>0.3</v>
@@ -22204,7 +22201,7 @@
         <v>0.6</v>
       </c>
       <c r="I25" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="26" spans="2:9">
@@ -22227,7 +22224,7 @@
         <v>0.4</v>
       </c>
       <c r="I26" s="429" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="27" spans="2:9">
@@ -22240,7 +22237,7 @@
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="442" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C28" s="439"/>
       <c r="D28" s="439"/>
@@ -22250,7 +22247,7 @@
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="437" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C29" s="434">
         <v>0.45</v>
@@ -22270,7 +22267,7 @@
     </row>
     <row r="30" spans="2:9">
       <c r="B30" s="437" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C30" s="434">
         <v>0.5</v>
@@ -22290,7 +22287,7 @@
     </row>
     <row r="31" spans="2:9">
       <c r="B31" s="437" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C31" s="434">
         <v>0.05</v>
@@ -22318,7 +22315,7 @@
     </row>
     <row r="33" spans="2:7" ht="28.5">
       <c r="B33" s="430" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C33" s="439"/>
       <c r="D33" s="439"/>
@@ -22328,7 +22325,7 @@
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="432" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C34" s="434">
         <v>0.8</v>
@@ -22348,7 +22345,7 @@
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="437" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C35" s="434">
         <v>0.2</v>
@@ -22376,7 +22373,7 @@
     </row>
     <row r="37" spans="2:7">
       <c r="B37" s="444" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C37" s="439"/>
       <c r="D37" s="439"/>
@@ -22386,7 +22383,7 @@
     </row>
     <row r="38" spans="2:7">
       <c r="B38" s="432" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C38" s="434">
         <v>0.05</v>
@@ -22406,7 +22403,7 @@
     </row>
     <row r="39" spans="2:7" ht="28.5">
       <c r="B39" s="432" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C39" s="434">
         <v>0.7</v>
@@ -22426,7 +22423,7 @@
     </row>
     <row r="40" spans="2:7" ht="28.5">
       <c r="B40" s="432" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C40" s="434">
         <v>0.2</v>
@@ -22454,7 +22451,7 @@
     </row>
     <row r="42" spans="2:7">
       <c r="B42" s="430" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C42" s="439"/>
       <c r="D42" s="439"/>
@@ -22464,7 +22461,7 @@
     </row>
     <row r="43" spans="2:7">
       <c r="B43" s="432" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C43" s="434">
         <v>0.15</v>
@@ -22484,7 +22481,7 @@
     </row>
     <row r="44" spans="2:7">
       <c r="B44" s="445" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C44" s="434">
         <v>0.45</v>
@@ -22504,7 +22501,7 @@
     </row>
     <row r="45" spans="2:7">
       <c r="B45" s="445" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C45" s="434">
         <v>0.4</v>
@@ -22557,7 +22554,7 @@
     <row r="53" spans="2:7">
       <c r="B53" s="446"/>
       <c r="C53" s="792" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D53" s="793"/>
       <c r="E53" s="793"/>
@@ -22655,44 +22652,44 @@
   <sheetData>
     <row r="2" spans="2:10" ht="14.25">
       <c r="B2" s="481" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C2" s="768" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="14.25">
       <c r="C5" s="483" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H5" s="483" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="14.25">
       <c r="C6" s="484"/>
       <c r="D6" s="484" t="s">
+        <v>512</v>
+      </c>
+      <c r="E6" s="484" t="s">
         <v>513</v>
       </c>
-      <c r="E6" s="484" t="s">
+      <c r="F6" s="763" t="s">
         <v>514</v>
       </c>
-      <c r="F6" s="763" t="s">
+      <c r="H6" s="484" t="s">
         <v>515</v>
       </c>
-      <c r="H6" s="484" t="s">
+      <c r="I6" s="484" t="s">
         <v>516</v>
       </c>
-      <c r="I6" s="484" t="s">
+      <c r="J6" s="484" t="s">
         <v>517</v>
-      </c>
-      <c r="J6" s="484" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="C7" s="484" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D7" s="485">
         <v>225</v>
@@ -22718,7 +22715,7 @@
     </row>
     <row r="8" spans="2:10">
       <c r="C8" s="484" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D8" s="485">
         <v>870</v>
@@ -22744,7 +22741,7 @@
     </row>
     <row r="9" spans="2:10" ht="14.25">
       <c r="C9" s="764" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D9" s="485">
         <v>496</v>
@@ -22770,7 +22767,7 @@
     </row>
     <row r="10" spans="2:10">
       <c r="C10" s="484" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D10" s="485">
         <v>780</v>
@@ -22796,7 +22793,7 @@
     </row>
     <row r="11" spans="2:10">
       <c r="C11" s="484" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D11" s="485">
         <v>199</v>
@@ -22822,7 +22819,7 @@
     </row>
     <row r="12" spans="2:10">
       <c r="C12" s="484" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D12" s="488">
         <v>1768</v>
@@ -22848,7 +22845,7 @@
     </row>
     <row r="13" spans="2:10">
       <c r="C13" s="484" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D13" s="485">
         <v>238</v>
@@ -22874,7 +22871,7 @@
     </row>
     <row r="14" spans="2:10" ht="14.25">
       <c r="C14" s="764" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D14" s="485">
         <v>347</v>
@@ -22975,7 +22972,7 @@
         <v>183.49097162510748</v>
       </c>
       <c r="G19" s="482" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="20" spans="3:10">
@@ -22986,19 +22983,19 @@
     </row>
     <row r="23" spans="3:10" ht="14.25">
       <c r="C23" s="489" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D23" s="484" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E23" s="484" t="s">
         <v>63</v>
       </c>
       <c r="H23" s="489" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I23" s="484" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J23" s="484" t="s">
         <v>63</v>
@@ -23006,7 +23003,7 @@
     </row>
     <row r="24" spans="3:10" ht="14.25">
       <c r="C24" s="485" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D24" s="484">
         <v>609</v>
@@ -23016,7 +23013,7 @@
         <v>0.12370505789152955</v>
       </c>
       <c r="H24" s="485" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I24" s="484">
         <v>539</v>
@@ -23028,7 +23025,7 @@
     </row>
     <row r="25" spans="3:10" ht="14.25">
       <c r="C25" s="485" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D25" s="484">
         <v>775</v>
@@ -23038,7 +23035,7 @@
         <v>0.15742433475523054</v>
       </c>
       <c r="H25" s="485" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I25" s="484">
         <v>461</v>
@@ -23050,7 +23047,7 @@
     </row>
     <row r="26" spans="3:10" ht="14.25">
       <c r="C26" s="485" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D26" s="484">
         <v>773</v>
@@ -23060,7 +23057,7 @@
         <v>0.15701807840747511</v>
       </c>
       <c r="H26" s="485" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I26" s="484">
         <v>309</v>
@@ -23072,7 +23069,7 @@
     </row>
     <row r="27" spans="3:10" ht="14.25">
       <c r="C27" s="485" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D27" s="484">
         <v>454</v>
@@ -23082,7 +23079,7 @@
         <v>9.2220190940483449E-2</v>
       </c>
       <c r="H27" s="485" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I27" s="484">
         <v>216</v>
@@ -23094,7 +23091,7 @@
     </row>
     <row r="28" spans="3:10" ht="14.25">
       <c r="C28" s="485" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D28" s="484">
         <v>883</v>
@@ -23104,7 +23101,7 @@
         <v>0.17936217753402398</v>
       </c>
       <c r="H28" s="484" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I28" s="484">
         <v>128</v>
@@ -23126,7 +23123,7 @@
         <v>8.1657525898842176E-2</v>
       </c>
       <c r="H29" s="767" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I29" s="484">
         <v>50</v>
@@ -23138,7 +23135,7 @@
     </row>
     <row r="30" spans="3:10" ht="14.25">
       <c r="C30" s="767" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D30" s="484">
         <v>356</v>
@@ -23148,7 +23145,7 @@
         <v>7.2313629900467191E-2</v>
       </c>
       <c r="H30" s="484" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I30" s="484">
         <v>41</v>
@@ -23170,7 +23167,7 @@
         <v>3.6156814950233596E-2</v>
       </c>
       <c r="H31" s="485" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I31" s="484">
         <v>10</v>
@@ -23182,7 +23179,7 @@
     </row>
     <row r="32" spans="3:10" ht="14.25">
       <c r="C32" s="485" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D32" s="484">
         <v>147</v>
@@ -23192,7 +23189,7 @@
         <v>2.9859841560024376E-2</v>
       </c>
       <c r="H32" s="767" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I32" s="484">
         <v>3</v>
@@ -23204,7 +23201,7 @@
     </row>
     <row r="33" spans="3:10">
       <c r="C33" s="485" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D33" s="484">
         <v>346</v>
@@ -23235,7 +23232,7 @@
     </row>
     <row r="36" spans="3:10" ht="14.25">
       <c r="C36" s="481" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D36" s="481">
         <f>SUM(D24:D27)</f>
@@ -23248,7 +23245,7 @@
     </row>
     <row r="37" spans="3:10" ht="14.25">
       <c r="C37" s="481" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D37" s="481">
         <f>D28+D30+D329+D33+D32</f>
@@ -23498,7 +23495,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1">
       <c r="A1" s="798" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B1" s="798"/>
       <c r="C1" s="798"/>
@@ -23517,10 +23514,10 @@
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1">
       <c r="A2" s="459" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B2" s="472" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C2" s="459"/>
       <c r="D2" s="459"/>
@@ -23535,59 +23532,59 @@
       <c r="M2" s="459"/>
       <c r="N2" s="460"/>
       <c r="O2" s="461" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="33.75" customHeight="1">
       <c r="A3" s="770" t="s">
+        <v>446</v>
+      </c>
+      <c r="B3" s="771" t="s">
+        <v>414</v>
+      </c>
+      <c r="C3" s="771" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" s="771" t="s">
         <v>447</v>
       </c>
-      <c r="B3" s="771" t="s">
-        <v>415</v>
-      </c>
-      <c r="C3" s="771" t="s">
-        <v>414</v>
-      </c>
-      <c r="D3" s="771" t="s">
+      <c r="E3" s="771" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3" s="771" t="s">
         <v>448</v>
       </c>
-      <c r="E3" s="771" t="s">
-        <v>418</v>
-      </c>
-      <c r="F3" s="771" t="s">
+      <c r="G3" s="771" t="s">
         <v>449</v>
       </c>
-      <c r="G3" s="771" t="s">
+      <c r="H3" s="771" t="s">
         <v>450</v>
       </c>
-      <c r="H3" s="771" t="s">
+      <c r="I3" s="771" t="s">
         <v>451</v>
       </c>
-      <c r="I3" s="771" t="s">
+      <c r="J3" s="771" t="s">
         <v>452</v>
       </c>
-      <c r="J3" s="771" t="s">
+      <c r="K3" s="771" t="s">
         <v>453</v>
       </c>
-      <c r="K3" s="771" t="s">
+      <c r="L3" s="771" t="s">
         <v>454</v>
       </c>
-      <c r="L3" s="771" t="s">
+      <c r="M3" s="771" t="s">
         <v>455</v>
       </c>
-      <c r="M3" s="771" t="s">
+      <c r="N3" s="771" t="s">
+        <v>433</v>
+      </c>
+      <c r="O3" s="771" t="s">
         <v>456</v>
-      </c>
-      <c r="N3" s="771" t="s">
-        <v>434</v>
-      </c>
-      <c r="O3" s="771" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1">
       <c r="A4" s="774" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B4" s="772">
         <v>435</v>
@@ -23634,7 +23631,7 @@
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1">
       <c r="A5" s="774" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B5" s="772">
         <v>362</v>
@@ -23681,7 +23678,7 @@
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1">
       <c r="A6" s="774" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B6" s="772">
         <v>265</v>
@@ -23728,7 +23725,7 @@
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1">
       <c r="A7" s="774" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B7" s="772">
         <v>224</v>
@@ -23775,7 +23772,7 @@
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1">
       <c r="A8" s="774" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B8" s="772">
         <v>284</v>
@@ -23822,7 +23819,7 @@
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1">
       <c r="A9" s="774" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B9" s="772">
         <v>324</v>
@@ -23869,7 +23866,7 @@
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1">
       <c r="A10" s="774" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B10" s="772">
         <v>353</v>
@@ -23916,7 +23913,7 @@
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1">
       <c r="A11" s="774" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B11" s="772">
         <v>305</v>
@@ -23963,7 +23960,7 @@
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1">
       <c r="A12" s="774" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B12" s="772">
         <v>235</v>
@@ -24010,7 +24007,7 @@
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1">
       <c r="A13" s="774" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B13" s="772">
         <v>301</v>
@@ -24057,7 +24054,7 @@
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1">
       <c r="A14" s="774" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B14" s="772">
         <v>298</v>
@@ -24104,7 +24101,7 @@
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1">
       <c r="A15" s="774" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B15" s="772">
         <v>294</v>
@@ -24151,7 +24148,7 @@
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1">
       <c r="A16" s="774" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B16" s="772">
         <v>218</v>
@@ -24198,7 +24195,7 @@
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1">
       <c r="A17" s="774" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B17" s="772">
         <v>221</v>
@@ -24245,7 +24242,7 @@
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1">
       <c r="A18" s="774" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B18" s="772">
         <v>375</v>
@@ -24275,7 +24272,7 @@
         <v>132</v>
       </c>
       <c r="K18" s="775" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="L18" s="772">
         <v>736</v>
@@ -24292,7 +24289,7 @@
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
       <c r="A19" s="774" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B19" s="772">
         <v>289</v>
@@ -24339,7 +24336,7 @@
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
       <c r="A20" s="774" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B20" s="772">
         <v>265</v>
@@ -24386,7 +24383,7 @@
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
       <c r="A21" s="774" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B21" s="772">
         <v>253</v>
@@ -24433,7 +24430,7 @@
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
       <c r="A22" s="774" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B22" s="772">
         <v>287</v>
@@ -24480,7 +24477,7 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1">
       <c r="A23" s="774" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B23" s="772">
         <v>293</v>
@@ -24527,7 +24524,7 @@
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
       <c r="A24" s="774" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B24" s="772">
         <v>268</v>
@@ -24574,7 +24571,7 @@
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
       <c r="A25" s="774" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B25" s="772">
         <v>618</v>
@@ -24621,7 +24618,7 @@
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
       <c r="A26" s="774" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B26" s="772">
         <v>285</v>
@@ -24668,7 +24665,7 @@
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1">
       <c r="A27" s="774" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B27" s="772">
         <v>287</v>
@@ -24715,7 +24712,7 @@
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1">
       <c r="A28" s="774" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B28" s="772">
         <v>233</v>
@@ -24739,7 +24736,7 @@
         <v>878</v>
       </c>
       <c r="I28" s="775" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="J28" s="772">
         <v>396</v>
@@ -24751,7 +24748,7 @@
         <v>1298</v>
       </c>
       <c r="M28" s="775" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="N28" s="772">
         <v>55</v>
@@ -24762,7 +24759,7 @@
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1">
       <c r="A29" s="774" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B29" s="772">
         <v>261</v>
@@ -24809,7 +24806,7 @@
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1">
       <c r="A30" s="774" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B30" s="772">
         <v>278</v>
@@ -24856,7 +24853,7 @@
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1">
       <c r="A31" s="774" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B31" s="772">
         <v>317</v>
@@ -24903,7 +24900,7 @@
     </row>
     <row r="32" spans="1:15" ht="15" customHeight="1">
       <c r="A32" s="774" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B32" s="772">
         <v>227</v>
@@ -24950,7 +24947,7 @@
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1">
       <c r="A33" s="774" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B33" s="772">
         <v>249</v>
@@ -24997,7 +24994,7 @@
     </row>
     <row r="34" spans="1:15" ht="15" customHeight="1">
       <c r="A34" s="774" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B34" s="772">
         <v>308</v>
@@ -25061,7 +25058,7 @@
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1">
       <c r="A36" s="776" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B36" s="777">
         <v>302</v>
@@ -25108,7 +25105,7 @@
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1">
       <c r="A37" s="800" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B37" s="800"/>
       <c r="C37" s="800"/>
@@ -25172,7 +25169,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="14.25">
       <c r="A2" s="769" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
   </sheetData>
@@ -25208,7 +25205,7 @@
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="555" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C3" s="556" t="s">
         <v>232</v>
@@ -25216,10 +25213,10 @@
     </row>
     <row r="4" spans="2:3">
       <c r="B4" s="558" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C4" s="558" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -25259,7 +25256,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="559" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="2:3">
@@ -25288,7 +25285,7 @@
     </row>
     <row r="13" spans="2:3">
       <c r="B13" s="559" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C13" s="559" t="s">
         <v>230</v>
@@ -25307,7 +25304,7 @@
     </row>
     <row r="16" spans="2:3" ht="18">
       <c r="B16" s="562" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C16" s="563"/>
     </row>
@@ -25329,7 +25326,7 @@
     </row>
     <row r="20" spans="2:3" ht="18">
       <c r="B20" s="566" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C20" s="567"/>
     </row>
@@ -25347,7 +25344,7 @@
     </row>
     <row r="24" spans="2:3" ht="18">
       <c r="B24" s="566" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C24" s="567"/>
     </row>
@@ -25356,7 +25353,7 @@
         <v>152</v>
       </c>
       <c r="C25" s="564" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="26" spans="2:3">
@@ -25372,12 +25369,12 @@
         <v>154</v>
       </c>
       <c r="C27" s="568" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="28" spans="2:3">
       <c r="B28" s="572" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C28" s="569">
         <v>2012</v>
@@ -25550,13 +25547,13 @@
     </row>
     <row r="5" spans="1:30" ht="14.25">
       <c r="A5" s="481" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C5" s="802" t="s">
         <v>262</v>
       </c>
       <c r="D5" s="802" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E5" s="801" t="str">
         <f>A11</f>
@@ -25665,7 +25662,7 @@
     </row>
     <row r="6" spans="1:30" ht="14.25">
       <c r="A6" s="481" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C6" s="801" t="str">
         <f>C5</f>
@@ -25782,7 +25779,7 @@
     </row>
     <row r="7" spans="1:30" ht="14.25">
       <c r="A7" s="481" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C7" s="801" t="str">
         <f>"*"&amp;C5</f>
@@ -25899,223 +25896,223 @@
     </row>
     <row r="10" spans="1:30" ht="14.65" thickBot="1">
       <c r="A10" s="803" t="s">
+        <v>616</v>
+      </c>
+      <c r="B10" s="803" t="s">
         <v>617</v>
-      </c>
-      <c r="B10" s="803" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="804" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B11" s="804" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="805" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B12" s="805" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="805" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B13" s="805" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="805" t="s">
+        <v>621</v>
+      </c>
+      <c r="B14" s="805" t="s">
         <v>622</v>
-      </c>
-      <c r="B14" s="805" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="805" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B15" s="805" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="805" t="s">
+        <v>624</v>
+      </c>
+      <c r="B16" s="805" t="s">
         <v>625</v>
-      </c>
-      <c r="B16" s="805" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="805" t="s">
+        <v>626</v>
+      </c>
+      <c r="B17" s="805" t="s">
         <v>627</v>
-      </c>
-      <c r="B17" s="805" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="805" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B18" s="805" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="805" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B19" s="805" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="805" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B20" s="805" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="805" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B21" s="805" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="805" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B22" s="805" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="805" t="s">
+        <v>633</v>
+      </c>
+      <c r="B23" s="805" t="s">
         <v>634</v>
-      </c>
-      <c r="B23" s="805" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="805" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B24" s="805" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="805" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B25" s="805" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="805" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B26" s="805" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="805" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B27" s="805" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="805" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B28" s="805" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="805" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B29" s="805" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="805" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B30" s="805" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="805" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B31" s="805" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="805" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B32" s="805" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="805" t="s">
+        <v>644</v>
+      </c>
+      <c r="B33" s="805" t="s">
         <v>645</v>
-      </c>
-      <c r="B33" s="805" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="805" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B34" s="805" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="805" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B35" s="805" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="805" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B36" s="805" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25">
       <c r="A37" s="806" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -26162,11 +26159,11 @@
   <dimension ref="A1:AO70"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B21" sqref="B21"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
-      <selection pane="bottomRight" activeCell="AK61" sqref="AK61"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.15"/>
@@ -26211,7 +26208,7 @@
   <sheetData>
     <row r="1" spans="1:41" s="240" customFormat="1" ht="105.75" customHeight="1" thickBot="1">
       <c r="A1" s="230" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B1" s="231" t="s">
         <v>263</v>
@@ -31770,7 +31767,7 @@
     </row>
     <row r="65" spans="1:39" ht="12.75" customHeight="1">
       <c r="A65" s="752" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B65" s="322"/>
       <c r="C65" s="323"/>
@@ -31813,7 +31810,7 @@
     </row>
     <row r="66" spans="1:39" ht="12.75" customHeight="1">
       <c r="A66" s="753" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B66" s="327"/>
       <c r="C66" s="323"/>
@@ -31856,7 +31853,7 @@
     </row>
     <row r="67" spans="1:39" ht="12.75" customHeight="1">
       <c r="A67" s="754" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B67" s="328"/>
       <c r="C67" s="323"/>
@@ -31899,7 +31896,7 @@
     </row>
     <row r="68" spans="1:39" ht="12.75" customHeight="1">
       <c r="A68" s="755" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B68" s="328"/>
       <c r="C68" s="323"/>
@@ -32000,8 +31997,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:BM72"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.15"/>
@@ -32303,7 +32300,7 @@
         <v>52</v>
       </c>
       <c r="I9" s="391" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="J9" s="391" t="s">
         <v>6</v>
@@ -32550,7 +32547,7 @@
     </row>
     <row r="16" spans="2:65" ht="18">
       <c r="B16" s="386" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C16" s="393"/>
       <c r="D16" s="393"/>
@@ -33750,7 +33747,7 @@
         <v>143</v>
       </c>
       <c r="Q50" s="350" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="T50" s="65"/>
       <c r="U50" s="378"/>
@@ -33767,7 +33764,7 @@
     </row>
     <row r="52" spans="2:21" ht="18">
       <c r="B52" s="363" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C52" s="386"/>
       <c r="D52" s="386"/>
@@ -33795,7 +33792,7 @@
     </row>
     <row r="54" spans="2:21">
       <c r="B54" s="353" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C54" s="352">
         <f>SUM('Commercial SEAI'!C6:G6)/1000</f>
@@ -33903,7 +33900,7 @@
     </row>
     <row r="62" spans="2:21" ht="14.25">
       <c r="B62" s="353" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C62" s="467">
         <f>C54*SUMPRODUCT('Commercial SEAI'!C6:G6,'Commercial SEAI'!C8:G8)/SUM('Commercial SEAI'!C6:G6)</f>
@@ -33973,7 +33970,7 @@
     </row>
     <row r="68" spans="2:9" ht="18">
       <c r="B68" s="363" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C68" s="364"/>
       <c r="D68" s="364"/>
@@ -33988,13 +33985,13 @@
         <v>95</v>
       </c>
       <c r="D69" s="353" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E69" s="466"/>
     </row>
     <row r="70" spans="2:9">
       <c r="B70" s="353" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C70" s="352">
         <f>C62*D70</f>
@@ -34049,8 +34046,8 @@
   </sheetPr>
   <dimension ref="B2:J40"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -34210,7 +34207,7 @@
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
@@ -34289,19 +34286,17 @@
         <v>211</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H14" s="29"/>
-      <c r="I14" s="29" t="s">
-        <v>386</v>
-      </c>
+      <c r="I14" s="29"/>
       <c r="J14" s="25"/>
     </row>
     <row r="15" spans="2:10">
@@ -34317,7 +34312,7 @@
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H15" s="29"/>
       <c r="I15" s="5"/>
@@ -34341,7 +34336,7 @@
     <row r="17" spans="2:9">
       <c r="B17" s="26"/>
       <c r="C17" s="27" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>105</v>
@@ -34373,17 +34368,17 @@
     <row r="19" spans="2:9">
       <c r="B19" s="26"/>
       <c r="C19" s="583" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D19" s="584" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E19" s="585" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="585"/>
       <c r="G19" s="29" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H19" s="29"/>
       <c r="I19" s="29"/>
@@ -34391,17 +34386,17 @@
     <row r="20" spans="2:9">
       <c r="B20" s="30"/>
       <c r="C20" s="588" t="s">
+        <v>545</v>
+      </c>
+      <c r="D20" s="588" t="s">
         <v>546</v>
-      </c>
-      <c r="D20" s="588" t="s">
-        <v>547</v>
       </c>
       <c r="E20" s="587" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="587"/>
       <c r="G20" s="24" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
@@ -34411,10 +34406,10 @@
         <v>134</v>
       </c>
       <c r="C21" s="582" t="s">
+        <v>551</v>
+      </c>
+      <c r="D21" s="582" t="s">
         <v>552</v>
-      </c>
-      <c r="D21" s="582" t="s">
-        <v>553</v>
       </c>
       <c r="E21" s="228" t="s">
         <v>10</v>
@@ -34427,10 +34422,10 @@
     <row r="22" spans="2:9">
       <c r="B22" s="26"/>
       <c r="C22" s="582" t="s">
+        <v>553</v>
+      </c>
+      <c r="D22" s="582" t="s">
         <v>554</v>
-      </c>
-      <c r="D22" s="582" t="s">
-        <v>555</v>
       </c>
       <c r="E22" s="228" t="s">
         <v>10</v>
@@ -34547,7 +34542,7 @@
         <v>CHCS</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>10</v>
@@ -34564,7 +34559,7 @@
         <v>CHPS</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>10</v>
@@ -34581,7 +34576,7 @@
         <v>CCCS</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>10</v>
@@ -34598,7 +34593,7 @@
         <v>CCPS</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>10</v>
@@ -34615,7 +34610,7 @@
         <v>CWCS</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>10</v>
@@ -34632,7 +34627,7 @@
         <v>CWPS</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>10</v>
@@ -34648,7 +34643,7 @@
         <v>57</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E35" s="29" t="s">
         <v>10</v>
@@ -34664,7 +34659,7 @@
         <v>58</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E36" s="29" t="s">
         <v>10</v>
@@ -34680,7 +34675,7 @@
         <v>59</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>10</v>
@@ -34696,7 +34691,7 @@
         <v>60</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E38" s="29" t="s">
         <v>10</v>
@@ -34712,7 +34707,7 @@
         <v>61</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E39" s="29" t="s">
         <v>10</v>
@@ -34728,7 +34723,7 @@
         <v>62</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>10</v>
@@ -36158,7 +36153,7 @@
         <v>10</v>
       </c>
       <c r="F70" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G70" s="54"/>
       <c r="H70" s="54"/>
@@ -36178,7 +36173,7 @@
         <v>10</v>
       </c>
       <c r="F71" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G71" s="54"/>
       <c r="H71" s="54"/>
@@ -36198,7 +36193,7 @@
         <v>10</v>
       </c>
       <c r="F72" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G72" s="54"/>
       <c r="H72" s="54"/>
@@ -36218,7 +36213,7 @@
         <v>10</v>
       </c>
       <c r="F73" s="55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G73" s="55"/>
       <c r="H73" s="55"/>
@@ -36240,7 +36235,7 @@
         <v>10</v>
       </c>
       <c r="F74" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G74" s="54"/>
       <c r="H74" s="54"/>
@@ -36260,7 +36255,7 @@
         <v>10</v>
       </c>
       <c r="F75" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G75" s="54"/>
       <c r="H75" s="54"/>
@@ -36280,7 +36275,7 @@
         <v>10</v>
       </c>
       <c r="F76" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G76" s="54"/>
       <c r="H76" s="54"/>
@@ -36300,7 +36295,7 @@
         <v>10</v>
       </c>
       <c r="F77" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G77" s="54"/>
       <c r="H77" s="54"/>
@@ -36320,7 +36315,7 @@
         <v>10</v>
       </c>
       <c r="F78" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G78" s="54"/>
       <c r="H78" s="54"/>
@@ -36340,7 +36335,7 @@
         <v>10</v>
       </c>
       <c r="F79" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G79" s="54"/>
       <c r="H79" s="54"/>
@@ -36360,7 +36355,7 @@
         <v>10</v>
       </c>
       <c r="F80" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G80" s="54"/>
       <c r="H80" s="54"/>
@@ -36380,7 +36375,7 @@
         <v>10</v>
       </c>
       <c r="F81" s="55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G81" s="55"/>
       <c r="H81" s="55"/>
@@ -36402,7 +36397,7 @@
         <v>10</v>
       </c>
       <c r="F82" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G82" s="54"/>
       <c r="H82" s="54"/>
@@ -36422,7 +36417,7 @@
         <v>10</v>
       </c>
       <c r="F83" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G83" s="57"/>
       <c r="H83" s="57"/>
@@ -36442,7 +36437,7 @@
         <v>10</v>
       </c>
       <c r="F84" s="55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G84" s="55"/>
       <c r="H84" s="55"/>
@@ -36464,7 +36459,7 @@
         <v>10</v>
       </c>
       <c r="F85" s="59" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G85" s="59"/>
       <c r="H85" s="59"/>
@@ -36486,7 +36481,7 @@
         <v>10</v>
       </c>
       <c r="F86" s="55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G86" s="55"/>
       <c r="H86" s="55"/>
@@ -36557,7 +36552,7 @@
         <v>113</v>
       </c>
       <c r="G89" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H89" s="53"/>
       <c r="I89" s="53"/>
@@ -36576,7 +36571,7 @@
         <v>10</v>
       </c>
       <c r="F90" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G90" s="54"/>
       <c r="H90" s="54"/>
@@ -36596,7 +36591,7 @@
         <v>10</v>
       </c>
       <c r="F91" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G91" s="54"/>
       <c r="H91" s="54"/>
@@ -36616,7 +36611,7 @@
         <v>10</v>
       </c>
       <c r="F92" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G92" s="54"/>
       <c r="H92" s="54"/>
@@ -36636,10 +36631,10 @@
         <v>10</v>
       </c>
       <c r="F93" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G93" s="54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H93" s="54"/>
       <c r="I93" s="54"/>
@@ -36658,7 +36653,7 @@
         <v>10</v>
       </c>
       <c r="F94" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G94" s="54"/>
       <c r="H94" s="54"/>
@@ -36678,10 +36673,10 @@
         <v>10</v>
       </c>
       <c r="F95" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G95" s="54" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H95" s="54"/>
       <c r="I95" s="54"/>
@@ -36700,7 +36695,7 @@
         <v>10</v>
       </c>
       <c r="F96" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G96" s="54"/>
       <c r="H96" s="54"/>
@@ -36720,7 +36715,7 @@
         <v>10</v>
       </c>
       <c r="F97" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G97" s="54"/>
       <c r="H97" s="54"/>
@@ -36740,7 +36735,7 @@
         <v>10</v>
       </c>
       <c r="F98" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G98" s="54"/>
       <c r="H98" s="54"/>
@@ -36760,7 +36755,7 @@
         <v>10</v>
       </c>
       <c r="F99" s="57" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G99" s="54"/>
       <c r="H99" s="54"/>
@@ -36843,10 +36838,10 @@
         <v>208</v>
       </c>
       <c r="H4" s="782" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I4" s="757" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="J4" s="514" t="s">
         <v>212</v>
@@ -36868,16 +36863,16 @@
       <c r="F5" s="516"/>
       <c r="G5" s="516"/>
       <c r="H5" s="784" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I5" s="516" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="J5" s="517" t="s">
         <v>213</v>
       </c>
       <c r="K5" s="517" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L5" s="516" t="s">
         <v>258</v>
@@ -36922,7 +36917,7 @@
       <c r="B7" s="518"/>
       <c r="C7" s="518"/>
       <c r="D7" s="519" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E7" s="520"/>
       <c r="F7" s="519"/>
@@ -37023,7 +37018,7 @@
         <v>COMGAS_INF</v>
       </c>
       <c r="C11" s="533" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D11" s="523" t="s">
         <v>185</v>
@@ -37087,10 +37082,10 @@
         <v>COMBGS_INF</v>
       </c>
       <c r="C13" s="525" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D13" s="525" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E13" s="527" t="str">
         <f>COM_Balance!$I$13</f>
@@ -37325,7 +37320,7 @@
         <v>81</v>
       </c>
       <c r="G26" s="757" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H26" s="513" t="s">
         <v>210</v>
@@ -37366,7 +37361,7 @@
         <v>COMHET_INF</v>
       </c>
       <c r="C28" s="586" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D28" s="541" t="s">
         <v>375</v>
@@ -37621,7 +37616,7 @@
         <v>81</v>
       </c>
       <c r="G42" s="757" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H42" s="513" t="s">
         <v>210</v>
@@ -37662,10 +37657,10 @@
         <v>COMH2G_INF</v>
       </c>
       <c r="C44" s="586" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E44" s="506" t="str">
         <f>COM_Commodities!C19</f>
@@ -37687,10 +37682,10 @@
         <v>COMH2L_INF</v>
       </c>
       <c r="C45" s="586" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E45" s="506" t="str">
         <f>COM_Commodities!C20</f>

</xml_diff>

<commit_message>
Reduce existing electricity demand in COM by DC amount
</commit_message>
<xml_diff>
--- a/VT_IE_COM.xlsx
+++ b/VT_IE_COM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF53B0FC-C715-464D-BE1A-4338DBC42ED2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47244CC-989D-4430-A842-D6BBDAF62F8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3233" yWindow="8002" windowWidth="20716" windowHeight="13276" tabRatio="891" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="33" r:id="rId1"/>
@@ -10126,8 +10126,8 @@
   </sheetPr>
   <dimension ref="B1:X171"/>
   <sheetViews>
-    <sheetView topLeftCell="D33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -16759,8 +16759,8 @@
   </sheetPr>
   <dimension ref="B1:Z91"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -17010,11 +17010,11 @@
       </c>
       <c r="D11" s="179">
         <f>K62*J60</f>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="E11" s="179">
         <f t="shared" si="0"/>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="F11" s="54" t="str">
         <f>COM_Commodities!E38</f>
@@ -18902,7 +18902,7 @@
       </c>
       <c r="J60" s="138">
         <f>R60</f>
-        <v>0.21907780602535418</v>
+        <v>0.11151590089149883</v>
       </c>
       <c r="K60" s="138">
         <f>S60</f>
@@ -18915,11 +18915,11 @@
       <c r="N60" s="69"/>
       <c r="O60" s="139">
         <f>IF(I60=0,0,K60*J60/I60)</f>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="P60" s="139">
         <f>COM_Balance!L46</f>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="Q60" s="203">
         <f>I60</f>
@@ -18927,7 +18927,7 @@
       </c>
       <c r="R60" s="73">
         <f>IF(S62=0,0,SUMPRODUCT(Q60,P60)/S62)</f>
-        <v>0.21907780602535418</v>
+        <v>0.11151590089149883</v>
       </c>
       <c r="S60" s="76">
         <f>IF($P$62*Q60=0,0,Q60*P60/SUMPRODUCT($P$60,$Q$60)*$S$62)</f>
@@ -18973,11 +18973,11 @@
       <c r="N62" s="69"/>
       <c r="O62" s="76">
         <f>SUM(O60)</f>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="P62" s="76">
         <f>SUM(P60)</f>
-        <v>15.911170581631776</v>
+        <v>8.0991705816317747</v>
       </c>
       <c r="Q62" s="165"/>
       <c r="R62" s="73"/>
@@ -21253,8 +21253,8 @@
   </sheetPr>
   <dimension ref="B3:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21843,7 +21843,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" ht="30">
       <c r="B9" s="329" t="s">
         <v>501</v>
       </c>
@@ -26100,12 +26100,12 @@
   </sheetPr>
   <dimension ref="A1:AS81"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="65" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="65" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B21" sqref="B21"/>
       <selection pane="topRight" activeCell="B21" sqref="B21"/>
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -33468,8 +33468,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:BM72"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -33952,7 +33952,7 @@
         <v>0.65641279696870891</v>
       </c>
       <c r="L12" s="277">
-        <f t="shared" si="0"/>
+        <f>SUM(L10:L11)</f>
         <v>42.679928352699655</v>
       </c>
       <c r="M12" s="277">
@@ -35088,8 +35088,8 @@
       <c r="J46" s="273"/>
       <c r="K46" s="273"/>
       <c r="L46" s="273">
-        <f>L$12*L25</f>
-        <v>15.911170581631776</v>
+        <f>L$12*L25-COM_DC!C7</f>
+        <v>8.0991705816317747</v>
       </c>
       <c r="M46" s="273"/>
       <c r="N46" s="251"/>
@@ -35156,7 +35156,7 @@
       </c>
       <c r="L48" s="272">
         <f t="shared" si="15"/>
-        <v>34.696483261115439</v>
+        <v>26.884483261115438</v>
       </c>
       <c r="M48" s="272">
         <f t="shared" si="15"/>
@@ -35168,7 +35168,7 @@
       </c>
       <c r="O48" s="135">
         <f>SUM(D48:N48)</f>
-        <v>35.537194895151437</v>
+        <v>27.725194895151439</v>
       </c>
       <c r="T48" s="65"/>
       <c r="U48" s="285"/>
@@ -35184,15 +35184,15 @@
       <c r="I49" s="258"/>
       <c r="O49" s="284">
         <f>O35+O38+O41+O48</f>
-        <v>72.097498869226484</v>
+        <v>64.285498869226501</v>
       </c>
       <c r="P49" s="257">
         <f>O49/3.6</f>
-        <v>20.027083019229579</v>
+        <v>17.857083019229584</v>
       </c>
       <c r="Q49" s="376">
         <f>O49/S5</f>
-        <v>1722.0191762020274</v>
+        <v>1535.432761756628</v>
       </c>
       <c r="T49" s="65"/>
       <c r="U49" s="285"/>
@@ -38831,8 +38831,8 @@
   </sheetPr>
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Specify CType for ELCC and DAYNITE for other electricity commodities and heat
</commit_message>
<xml_diff>
--- a/VT_IE_COM.xlsx
+++ b/VT_IE_COM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47244CC-989D-4430-A842-D6BBDAF62F8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B68F01-A76F-4FD1-A880-39E266E07762}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="891" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="33" r:id="rId1"/>
@@ -33468,7 +33468,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:BM72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
@@ -35517,8 +35517,8 @@
   </sheetPr>
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -35809,7 +35809,7 @@
       </c>
       <c r="G14" s="29"/>
       <c r="H14" s="29" t="s">
-        <v>378</v>
+        <v>75</v>
       </c>
       <c r="I14" s="29"/>
       <c r="J14" s="29"/>
@@ -40319,9 +40319,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -40471,19 +40474,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B89BCC-8A48-4F37-9079-7262C2133970}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBACB2E3-CDF0-4ED0-BEB9-5A15710DBCB9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -40507,9 +40506,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBACB2E3-CDF0-4ED0-BEB9-5A15710DBCB9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84B89BCC-8A48-4F37-9079-7262C2133970}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>